<commit_message>
xls: Add a summary of the learning knowledge in the past five days
</commit_message>
<xml_diff>
--- a/leetcode路线.xlsx
+++ b/leetcode路线.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18855" windowHeight="12495"/>
+    <workbookView windowWidth="14940" windowHeight="12390"/>
   </bookViews>
   <sheets>
     <sheet name="leetcode刷题" sheetId="1" r:id="rId1"/>
@@ -15,11 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="355">
-  <si>
-    <t>从8月2日开始保持每天2个题目,还剩204题,写102天,2024年11月12日可刷完leetcode第一遍
-从9.3日起,如果每天写3个题,写37天,2024 年 10 月 22 日就能写完第一遍
-从9.3日起,如果每天写4个题,写37天,2024 年 10 月 9 日就能写完第一遍
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="353">
+  <si>
+    <t>从9月23日开始保持每天2个题目,还剩113题,写57天,2024年11月19日可刷完leetcode第一遍
 慢慢做,不要慌,每个题都要搞懂,不要水,静下心来</t>
   </si>
   <si>
@@ -1307,9 +1305,6 @@
     <t>113. 路径总和 II</t>
   </si>
   <si>
-    <t>计划9.7日</t>
-  </si>
-  <si>
     <t>js:
 这个题迭代方法不好写,要记录每条路径很麻烦
 递归方法-要遍历整个树,找到所有路径,所以递归函数不要返回值!
@@ -1373,9 +1368,6 @@
   </si>
   <si>
     <t>98. 验证二叉搜索树</t>
-  </si>
-  <si>
-    <t>计划9.8</t>
   </si>
   <si>
     <t>js:
@@ -1445,9 +1437,6 @@
   </si>
   <si>
     <t xml:space="preserve"> 701.二叉搜索树中的插入操作</t>
-  </si>
-  <si>
-    <t>计划9.9日</t>
   </si>
   <si>
     <t>js:
@@ -1540,9 +1529,6 @@
     <t>77. 组合</t>
   </si>
   <si>
-    <t>计划9.12日</t>
-  </si>
-  <si>
     <t>js:
 方案一: 回溯法, 抄的, 学习回溯算法,熟悉模板
 方案二: +剪枝操作
@@ -1568,9 +1554,6 @@
   </si>
   <si>
     <t>39. 组合总和</t>
-  </si>
-  <si>
-    <t>计划9.13日</t>
   </si>
   <si>
     <t>js:
@@ -1663,21 +1646,25 @@
     <t>47. 全排列 II</t>
   </si>
   <si>
-    <t>计划9.14日</t>
-  </si>
-  <si>
     <t>js:
 抄的, 题之间细微差别没搞清楚, 需要横向对比, 画图对比
 一般来说：组合问题和排列问题是在树形结构的叶子节点上收集结果，而子集问题就是取树上所有节点的结果</t>
   </si>
   <si>
+    <t>332. 重新安排行程</t>
+  </si>
+  <si>
+    <t>js:
+抄的，不会写，而且没过，超时</t>
+  </si>
+  <si>
     <t>棋盘问题</t>
   </si>
   <si>
+    <t>51. N 皇后</t>
+  </si>
+  <si>
     <t>其他</t>
-  </si>
-  <si>
-    <t>计划9.15日</t>
   </si>
   <si>
     <t>总结:
@@ -1701,19 +1688,25 @@
     <t>贪心算法22</t>
   </si>
   <si>
-    <t>计划9.16日</t>
-  </si>
-  <si>
-    <t>计划9.17日</t>
-  </si>
-  <si>
-    <t>计划9.18日</t>
-  </si>
-  <si>
-    <t>计划9.19日</t>
-  </si>
-  <si>
-    <t>计划9.20日</t>
+    <t>455. 分发饼干</t>
+  </si>
+  <si>
+    <t>js:
+本来很快就能写出来!结果,被sort摆了一道,气死我了!!!
+g.sort()：按照字符串的Unicode码点顺序进行排序。因此结果可能并不是按数值的大小进行排序。
+g.sort((a, b) =&gt; a - b)：带有比较函数的排序方式，能够按照数值的大小对数组元素进行排序。
+    (a, b) =&gt; a - b 是一个比较函数，当 a - b 为负数时，a 会排在 b 之前，这就能保证数字按升序排列。</t>
+  </si>
+  <si>
+    <t>9.23总结:
+1.什么是贪心: 本质是选择每一阶段的局部最优, 从而达到全局最优
+2.什么时候使用贪心:  刷题或者面试的时候，手动模拟一下感觉可以局部最优推出整体最优，而且想不到反例，那么就试一试贪心. 贪心没有套路，说白了就是常识性推导加上举反例
+3.贪心算法一般分为如下四步：
+    将问题分解为若干个子问题
+    找出适合的贪心策略
+    求解每一个子问题的最优解
+    将局部最优解堆叠成全局最优解
+做题的时候，只要想清楚 局部最优 是什么，如果推导出全局最优，其实就够了。</t>
   </si>
   <si>
     <t>动态规划52</t>
@@ -1722,13 +1715,176 @@
     <t>单调栈5</t>
   </si>
   <si>
-    <t>计划9.21日</t>
-  </si>
-  <si>
     <t>图论30</t>
   </si>
   <si>
     <t>2024/9/2 4:48:00+74</t>
+  </si>
+  <si>
+    <t>项目学习</t>
+  </si>
+  <si>
+    <t>js实现jquery</t>
+  </si>
+  <si>
+    <t>9.19-9.23</t>
+  </si>
+  <si>
+    <t>1.DOMContentLoaded: 当 HTML 文档完全解析，且所有延迟脚本（&lt;script defer src="…"&gt; 和 &lt;script type="module"&gt;）下载和执行完毕后，会触发 DOMContentLoaded 事件。它不会等待图片、子框架和异步脚本等其他内容完成加载。DOMContentLoaded 是一个不冒泡的事件。这意味着它只会在 document 对象上触发，而不会从 document 冒泡到 window 或其他元素。因此，不存在像常规冒泡事件（如 click、submit 等）那样的冒泡传播问题。
+2. DOM 事件模型中，事件的传播分为三个主要阶段：
+    捕获阶段：事件从文档的根节点开始，向下传播到目标元素。
+    目标阶段：事件到达目标元素，即事件所直接作用的元素。
+    冒泡阶段：事件从目标元素开始，向上传播到根节点（或父级元素）(解决方案: stopPropogation)
+举例:
+&lt;div id="parent"&gt;
+  &lt;button id="child"&gt;Click me&lt;/button&gt;
+&lt;/div&gt;
+    捕获阶段：
+        window → document → html → body → div#parent → button#child（但事件处理程序不会在目标元素 button 处触发，只是在它的祖先元素上触发，且需要设置 capture: true 才能捕获）
+    目标阶段：
+        事件到达目标元素 button#child，触发绑定在该元素上的监听器（无论是捕获阶段还是冒泡阶段的监听器）
+    冒泡阶段：
+        button#child → div#parent → body → html → document → window（在目标元素上的冒泡监听器触发，然后事件逐级往上冒泡）
+3.HTMLCollection 和 NodeList 的区别 &amp;&amp; 不能使用typeof判断类数组元素 &amp;&amp; 哪些元素获取器返回HTMLCollection,哪些返回NodeList &amp;&amp; jquery语法
+    a.HTMLCollection 和 NodeList 是两种不同的类数组集合，它们虽然都可以包含多个 DOM 元素，但本质上是不同的类型。
+       NodeList 对象是节点的集合，通常是由属性，如Node.childNodes 和 方法，如document.querySelectorAll 返回的
+    HTMLCollection：
+        动态更新：当文档中的元素被修改时，HTMLCollection 会自动反映这些更改。
+        返回方法：getElementsByClassName() 和 getElementsByTagName() 都返回 HTMLCollection 类型。
+    NodeList：
+        可以是静态或动态：NodeList 的内容可以是静态的，也可以动态更新。
+        返回方法：querySelectorAll() 返回的是 静态的 NodeList，而 childNodes 返回的是 动态的 NodeList。
+b.HTMLCollection 是一种类数组对象，用来表示一组 HTML 元素。它不是标准的 JavaScript 对象或数组，因此不能使用 typeof 来判断它。typeof 只能返回一些基本数据类型，如 string, number, object, function 等。对于 HTMLCollection，使用 typeof 结果会返回 "object"，但它和普通的 JavaScript 对象有明显的区别。HTMLCollection 不是一个真正的数组（例如，它没有数组的 forEach 方法），但它具有 length 属性，可以用 for 循环进行遍历。可以使用 instanceof 或 Array.isArray() 来进行判断. 通过 instanceof 来判断 this.arg 是否为 HTMLCollection 或 NodeList
+c.HTMLCollection 在某些环境中会被认为是 NodeList.
+d.getElementsByClassName和getElementsByTagName返回的是HTMLCollection, querySelectorAll返回的是NodeList, 由于浏览器的不一致行为,可能会导致getElementsByTagName
+4.运行测试器对比 JEST VS Karma
+Jest 是一个集成度更高、功能更丰富的测试运行器，适合Node.js 和现代前端框架（如 React、Vue）的单元测试。
+Karma 更适合需要在真实浏览器中运行的项目，尤其是在进行跨浏览器兼容性测试时。
+    Jest：
+        最初专注于 Node.js 环境，但通过 jsdom 支持浏览器测试。
+        内置功能丰富：Jest 内置了自动模拟、快照测试、并行运行测试、测试覆盖率等功能, 不需要额外配置断言库（如 Chai）或测试框架（如 Mocha），简化了测试配置和运行。
+        适合单元测试和小规模集成测试，配置简单且开箱即用，广受 React、Vue 等前端框架开发者的喜爱。
+        Jest 的测试速度较快，并且由于其强大的内置功能，很多开发者选择它来替代 Karma。
+    Karma：
+        浏览器测试为主：Karma 的一个重要特点是它能在真实浏览器中运行测试，因此更适合那些需要在多个浏览器中测试代码的项目。你可以通过 Karma 启动 Chrome、Firefox、Safari 等浏览器来运行测试。
+        纯测试运行器：Karma 专注于作为一个测试运行器，它本身不包含断言库或测试框架。Karma 需要结合其他测试框架和断言库使用，比如 Mocha、Jasmine 或 Chai。
+        更适合大规模的集成测试，特别是需要在不同浏览器中运行测试时。
+当前趋势
+    Jest 在现代前端开发中逐渐占据主导地位，但 Karma 在需要跨浏览器的测试场景中仍然有一定优势。如果主要在 Node.js 环境或不需要真实的浏览器运行，Jest 可能是更流行的选择。
+5.JEST:
+Jest 默认不支持 ES6 的模块语法（import/export）。在 Node.js 环境中，Jest 默认期望使用 CommonJS 模块语法（require）,如果要使用es模块,就要使用Babel转换成ES6语法, 除此之外, Jest 默认的测试环境不支持浏览器 API（如 document），因此你需要将测试环境设置为 jsdom，以便能够模拟浏览器环境 -&gt; 修改配置文件; 
+JEST测试结构:
+describe 块：用于组织相关的测试，便于分组和分类。
+test 或 it 块：每个测试用例，描述某个具体的功能。
+expect 函数：用于断言，验证函数的返回值是否符合预期。可以使用 toBe、toEqual、toContain 等多种断言方法。
+6.为什么 Karma 生成的配置文件使用 CommonJS 语法？
+    Karma 配置文件运行在 Node.js 中：
+        Karma 的配置文件（karma.conf.js）是在 Node.js 环境 下执行的，而不是在浏览器中运行的。Node.js 传统上使用 CommonJS 模块系统，因此 Karma 使用 CommonJS 语法来兼容大多数用户的开发环境。
+        当 Karma 运行时，它会启动一个 Node.js 服务器，并为浏览器提供测试文件。虽然浏览器可以处理 ES 模块，但 Karma 服务器的配置文件需要与 Node.js 的模块系统兼容。
+    向后兼容性和普遍性：
+        CommonJS 在 Node.js 中仍然是非常普遍的模块格式，因此 Karma 的默认配置使用这种格式来避免兼容性问题。这确保了它能在大多数项目中无缝运行，即便项目本身没有使用 ES 模块。
+    工具链和生态系统：
+        Karma 生态中很多插件（如 karma-webpack、karma-mocha）依然使用 CommonJS 规范进行模块管理。保持配置文件也使用 CommonJS，可以减少很多复杂的兼容性问题。
+7.测试工具学习建议:
+测试运行器（如 Mocha, Jest）：学习如何执行测试文件，了解测试生命周期（如 beforeEach、afterEach）。
+断言库（如 Chai, Jest 内置 expect）：学习如何编写断言，用于验证代码输出是否符合预期。
+测试框架：了解如何使用测试框架组织测试、分模块测试，以及如何进行异步测试。
+高级概念：学习如何进行性能测试、集成测试和端到端测试等。
+8.webpack是打包工具,和这里的测试运行器是什么关系,为什么需要一个打包工具帮助处理es模块,请详细解释
+之所以需要 Webpack 来帮助处理 ES 模块，主要是因为测试运行器（如 Karma）和浏览器本身并不能直接理解或运行未打包的 ES 模块文件。
+Karma 的作用是加载你的测试文件、运行测试，并把结果显示在终端或浏览器中，但它并不直接支持 ES 模块或其他现代 JavaScript 语法（例如 JSX、TypeScript、ES6+ 等）。原因: 1. 测试运行器的职责是启动浏览器并加载测试脚本，但并不理解或转换现代 JavaScript 语法。 2. 即便浏览器支持 ES 模块，但测试脚本和模块的加载方式可能会和打包环境有所不同。例如，如果你有多个模块文件，浏览器需要根据相对路径逐个加载它们，而 Karma 运行时只会加载单个入口文件（通常是测试文件），而不会自动加载相关依赖
+Webpack 在这里的作用
+Webpack 是一个模块打包工具，可以帮助你在运行测试之前将所有模块（包括测试文件及其依赖项）打包成一个文件，确保测试运行器和浏览器可以正确执行。这是通过以下方式实现的：
+    模块依赖管理：Webpack 解析 import 或 require 语句，将所有依赖的模块打包为一个或多个文件，解决了浏览器或测试运行器无法直接加载多个模块的问题。
+    转换代码：Webpack 能够配合 Babel 等工具，将 ES 模块转换为浏览器或测试环境能够识别的格式（例如 CommonJS 或 AMD 模块），并支持各种现代 JavaScript 语法。即使 Karma 不支持原生 ES 模块，Webpack 通过转换代码的方式保证测试代码能够运行。
+    预处理测试文件：在使用 Karma 运行测试时，Webpack 可以作为 Karma 的“预处理器”，即在 Karma 加载测试文件之前，先由 Webpack 对这些文件进行打包和转换，然后将打包后的文件交给 Karma 运行。
+Webpack 与 Karma 的工作流程
+当你在 Karma 中使用 Webpack 时，工作流程如下
+    Karma 启动：Karma 作为测试运行器启动，准备运行你的测试文件。
+    Webpack 预处理器：Karma 通过配置 Webpack 作为预处理器，在加载测试文件之前，Webpack 会根据 import 或 require 语句打包所有模块，并将所有依赖合并为一个文件。
+    浏览器运行：Webpack 完成打包后，Karma 会将生成的测试文件发送到浏览器中运行。浏览器不需要再单独加载和解析每个模块文件，而是一次性加载打包后的文件。
+    测试执行：浏览器中执行打包后的测试文件，Karma 收集测试结果并反馈到命令行或报告中。
+结论
+Webpack 在 Karma 测试环境中起到了关键作用，主要是通过：
+    解析和打包 ES 模块及其依赖。
+    转换现代 JavaScript 语法，使其兼容 Karma 和浏览器的测试环境。
+    提供预处理功能，在测试运行之前将测试代码打包为单个文件。
+Karma 本身默认支持 CommonJS 模块，因为它运行在 Node.js 环境中，并且插件和工具生态大多基于 CommonJS。
+ES 模块 支持依赖浏览器来处理，需要配置 Karma 和浏览器环境来支持 ES 模块的加载。
+使用 Webpack 或其他打包工具可以简化和增强对 ES 模块的支持，特别是当项目中使用大量 ES 模块时。
+9.使用webpack给Karma处理es模块的思路:
+1.Karma 使用 Webpack 作为预处理器： Karma 需要通过 Webpack 来处理 ES 模块，因此你要在 Karma 的配置中加入 Webpack 相关的设置。
+2.Webpack 专门为测试环境设置： 你可以使用部分和开发类似的 Webpack 配置，但需要根据测试需求简化或调整。
+10.Karma与Ci/CD的应用场景 &amp;&amp; 对比:
+Karma应用场景:
+适合前端开发人员在本地开发环境中执行单元测试或集成测试。
+提供跨浏览器的测试支持，确保代码在不同浏览器中的一致性。
+CI/CD应用场景:
+每当代码提交到远程仓库（如GitHub、GitLab等）时，CI/CD工具（如Jenkins、GitLab CI、Travis CI等）会自动拉取最新代码并运行预设的测试。
+测试可以包括单元测试、集成测试、端到端测试等。
+如果所有测试通过，CI/CD工具会将代码部署到特定的环境中。
+CI/CD和Karma的区别:
+    运行环境：
+        Karma测试：主要在本地或测试环境中使用，主要关注前端代码的正确性和跨浏览器兼容性。
+        CI/CD测试：主要在持续集成环境中自动执行，可能包括后端、数据库、API的测试。Karma测试可以是CI/CD流程中的一个步骤。
+    自动化程度：
+        Karma测试：可以手动或自动运行测试，通常与开发人员的日常工作结合。
+        CI/CD测试：完全自动化，通常触发代码提交或合并时运行。
+    范围：
+        Karma测试：通常是针对JavaScript代码的单元测试或前端集成测试。
+        CI/CD测试：包括单元测试、集成测试、端到端测试、性能测试，甚至包括Karma在内的多个测试工具。</t>
+  </si>
+  <si>
+    <t>小知识集锦:
+1.Node.js :是在服务器端运行 JavaScript 的环境，主要特点是基于事件驱动、异步 I/O，适合处理高并发场景
+2.js中匿名函数（和所有传统的 Javascript 函数）创建他们独有的 this 对象，而箭头函数则继承绑定他所在函数的 this 对象
+3. RegExp.prototype.test(): test() 方法执行一个检索，用来查看正则表达式与指定的字符串是否匹配。返回 true 或 false。
+4.jquery语法中$()括号中是可以传入NodeList类型内容,但是不能直接是HTMLCollection
+    语法: 以下这两种写法一样, 都是为了防止文档在完全加载（就绪）之前运行 jQuery 代码，即在 DOM 加载完成后才可以对 DOM 进行操作:
+$(document).ready(function(){
+   // 开始写 jQuery 代码...
+});
+$(function(){
+   // 开始写 jQuery 代码...
+});
+5.判断typeof的时候, ===右边应该是字符串: typeof arg === 'function'
+6.instanceof: instanceof 运算符用于检测构造函数的 prototype 属性是否出现在某个实例对象的原型链上。
+7. Object.entries(): 静态方法返回一个数组，包含给定对象自有的可枚举字符串键属性的键值对。可使用如下方法:
+for(const [key, value] of Object.entries(collections)) {
+    console.log(key, value);
+}
+8.npx 是什么: 一个工具，允许你在本地或全局安装的 node_modules 中执行包中的命令，而不需要将其全局安装。它简化了命令的调用，比如 eslint 或 webpack，无需手动安装到全局环境。
+9.断言: 是在测试中用于验证程序行为的一种表达。简单来说，断言就是检查某个值是否符合期望。如果断言成功（即条件为真），测试继续运行；如果断言失败，测试就会中断，并报告错误。
+在测试框架中，断言的目的是确保代码的行为符合预期。通常会有多种断言方法，用来检查不同类型的结果，比如值相等、对象相等、是否包含某个元素、函数是否抛出了异常等。
+10.Babel : 是一个 JavaScript 编译器，主要用于将现代 JavaScript 代码（如 ES6+、ES7、ES8 等）转换为向下兼容的旧版 JavaScript 代码，使得可以在不支持新特性的浏览器和环境中运行这些代码。
+babel-loader:这是 webpack 用来处理 Babel 转译 JavaScript 文件的加载器, @babel/preset-env 是 Babel 最常用的预设，用来将现代 JavaScript 代码转换为更兼容的版本
+11.Symbol不能使用this.SYM_NODE_LIST访问,使用this[SYM_NODE_LIST]才能访问. this.SYM_NODE_LIST: 这里 SYM_NODE_LIST 是一个普通的属性名，并且是以字符串形式存储的。它等价于 this['SYM_NODE_LIST'], SYM_NODE_LIST 是一个变量，它存储的是 Symbol('nodelist') 的值。Symbol 是一种创建独一无二的标识符的方式，因此 SYM_NODE_LIST 的值并不是字符串，而是一个 Symbol 类型的值。在使用 this[SYM_NODE_LIST] 时，你是在访问一个符号键的属性。通常用作对象的属性键，以确保属性的唯一性和不可冲突性。
+const SYM_NODE_LIST = Symbol('nodelist');  中的'nodelist' 作为描述仅用于标识这个 Symbol 与节点列表相关，但不参与代码逻辑中的行为，只是便于开发者理解。
+12.utils文件作用: 主要是抽象出独立于业务逻辑的工具方法
+13.'--save-dev 是 npm 命令中的一个选项，用于将指定的包（模块）作为 开发依赖 安装，并将其记录在 package.json 文件的 devDependencies 部分。
+14.CommonJS与ES Module:
+    CommonJS导入导出
+        require
+        module.exports
+        exports
+    ES Module导入导出
+        import
+        export
+        export default
+15.现代浏览器确实支持 ES6 模块（ESM）。但要使用 import 语句，必须确保在script中使用 type="module"
+16.webpack 和 webpack-cli 是 Webpack 的核心库，用于打包 JavaScript 文件。
+karma-webpack 是 Karma 与 Webpack 的整合插件，能够让 Karma 使用 Webpack 编译和打包文件。
+17.document.querySelectorAll('.test') 返回的是一个 NodeList 集合，而不是一个单一的 DOM 元素
+[...document.querySelectorAll(selector)]这样写就是普通数组
+18..js与.cjs的区别
+.js 文件在 "type": "module" 项目中表示 ES Module，而 .cjs 文件总是表示 CommonJS。
+语法：ESM 使用 import/export，而 CommonJS 使用 require/module.exports。
+兼容性：如果你的项目使用现代模块系统（如 ES6 模块），那么使用 .js；如果需要兼容旧的 CommonJS 模块，使用 .cjs
+19.CI/CD(是自动化集成测试的一部分，通常是软件交付流水线的一部分。CI（持续集成）指的是开发人员将代码频繁地合并到主分支，并在每次合并时自动运行一系列测试来验证代码的正确性。CD（持续交付/持续部署）则进一步自动化，将通过测试的代码部署到生产环境或预发布环境)
+20.在配置中的browsers: ['ChromeHeadless'],什么是无头模式:
+无头模式（Headless Mode）指的是运行浏览器时不显示图形界面的模式。它可以执行浏览器操作（如加载页面、执行JavaScript等），但不会在屏幕上显示出来。无头模式通常用于自动化测试、网络爬虫、CI/CD等场景，因为它更轻量、速度更快。
+在你的测试场景中，使用无头模式（如ChromeHeadless）可以通过Puppeteer控制浏览器来运行测试，而无需打开真实的浏览器窗口。
+21.同步任务按照顺序逐一执行，而异步任务在等待某些操作完成的同时，可以继续执行其他任务，不阻塞主线程</t>
   </si>
   <si>
     <t>已有书籍</t>
@@ -1773,8 +1929,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="0.00_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="yyyy/m/d;@"/>
@@ -1809,13 +1965,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -1824,15 +1973,30 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1846,7 +2010,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -1855,21 +2018,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1877,40 +2026,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1929,8 +2047,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1944,11 +2094,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1985,7 +2141,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1997,7 +2189,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2015,127 +2225,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2153,13 +2243,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2262,65 +2418,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2345,6 +2442,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2359,157 +2480,192 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2600,35 +2756,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2952,12 +3111,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G176"/>
+  <dimension ref="A1:G182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G135" sqref="G135"/>
+      <selection pane="bottomLeft" activeCell="G144" sqref="G144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="16.5" outlineLevelCol="6"/>
@@ -4702,7 +4861,7 @@
       <c r="E105" s="19" t="s">
         <v>258</v>
       </c>
-      <c r="F105" s="19"/>
+      <c r="F105" s="30"/>
       <c r="G105" s="12" t="s">
         <v>259</v>
       </c>
@@ -4718,11 +4877,9 @@
       <c r="E106" s="19">
         <v>9.7</v>
       </c>
-      <c r="F106" s="26" t="s">
+      <c r="F106" s="30"/>
+      <c r="G106" s="12" t="s">
         <v>261</v>
-      </c>
-      <c r="G106" s="12" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="107" ht="24" spans="2:7">
@@ -4730,17 +4887,17 @@
         <v>25</v>
       </c>
       <c r="C107" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D107" s="12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E107" s="19">
         <v>9.7</v>
       </c>
-      <c r="F107" s="28"/>
+      <c r="F107" s="30"/>
       <c r="G107" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="108" ht="60" spans="2:7">
@@ -4748,17 +4905,17 @@
         <v>26</v>
       </c>
       <c r="C108" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D108" s="12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E108" s="19">
         <v>9.7</v>
       </c>
-      <c r="F108" s="28"/>
+      <c r="F108" s="30"/>
       <c r="G108" s="12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="109" ht="120" spans="2:7">
@@ -4766,17 +4923,17 @@
         <v>27</v>
       </c>
       <c r="C109" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D109" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E109" s="19">
         <v>9.7</v>
       </c>
-      <c r="F109" s="28"/>
+      <c r="F109" s="30"/>
       <c r="G109" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="110" ht="48" spans="2:7">
@@ -4784,17 +4941,17 @@
         <v>28</v>
       </c>
       <c r="C110" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D110" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E110" s="19">
         <v>9.8</v>
       </c>
-      <c r="F110" s="28"/>
+      <c r="F110" s="30"/>
       <c r="G110" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="111" ht="132" spans="2:7">
@@ -4802,17 +4959,17 @@
         <v>29</v>
       </c>
       <c r="C111" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D111" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E111" s="19">
         <v>9.8</v>
       </c>
-      <c r="F111" s="29"/>
+      <c r="F111" s="30"/>
       <c r="G111" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="112" ht="72" spans="2:7">
@@ -4820,19 +4977,17 @@
         <v>30</v>
       </c>
       <c r="C112" s="10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D112" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E112" s="19">
         <v>9.8</v>
       </c>
-      <c r="F112" s="26" t="s">
-        <v>274</v>
-      </c>
+      <c r="F112" s="30"/>
       <c r="G112" s="12" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="113" ht="108" spans="2:7">
@@ -4840,17 +4995,17 @@
         <v>31</v>
       </c>
       <c r="C113" s="10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D113" s="12" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E113" s="19">
         <v>9.8</v>
       </c>
-      <c r="F113" s="28"/>
+      <c r="F113" s="30"/>
       <c r="G113" s="12" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="114" ht="156" spans="2:7">
@@ -4858,17 +5013,17 @@
         <v>32</v>
       </c>
       <c r="C114" s="10" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D114" s="12" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E114" s="19">
         <v>9.8</v>
       </c>
-      <c r="F114" s="28"/>
+      <c r="F114" s="30"/>
       <c r="G114" s="12" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="115" ht="276" spans="2:7">
@@ -4876,17 +5031,17 @@
         <v>33</v>
       </c>
       <c r="C115" s="10" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D115" s="12" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E115" s="19">
         <v>9.9</v>
       </c>
-      <c r="F115" s="28"/>
+      <c r="F115" s="30"/>
       <c r="G115" s="12" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="116" ht="96" spans="2:7">
@@ -4894,17 +5049,17 @@
         <v>34</v>
       </c>
       <c r="C116" s="10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D116" s="12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E116" s="19">
         <v>9.9</v>
       </c>
-      <c r="F116" s="29"/>
+      <c r="F116" s="30"/>
       <c r="G116" s="12" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="117" ht="72" spans="2:7">
@@ -4912,19 +5067,17 @@
         <v>35</v>
       </c>
       <c r="C117" s="10" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D117" s="12" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E117" s="19">
         <v>9.9</v>
       </c>
-      <c r="F117" s="26" t="s">
-        <v>285</v>
-      </c>
+      <c r="F117" s="30"/>
       <c r="G117" s="12" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="118" ht="96" spans="2:7">
@@ -4932,17 +5085,17 @@
         <v>36</v>
       </c>
       <c r="C118" s="10" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D118" s="12" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E118" s="19">
         <v>9.9</v>
       </c>
-      <c r="F118" s="28"/>
+      <c r="F118" s="30"/>
       <c r="G118" s="12" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="119" ht="24" spans="2:7">
@@ -4950,17 +5103,17 @@
         <v>37</v>
       </c>
       <c r="C119" s="10" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D119" s="12" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E119" s="19">
         <v>9.11</v>
       </c>
-      <c r="F119" s="28"/>
+      <c r="F119" s="30"/>
       <c r="G119" s="12" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="120" ht="72" spans="2:7">
@@ -4968,17 +5121,17 @@
         <v>38</v>
       </c>
       <c r="C120" s="10" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D120" s="12" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E120" s="19">
         <v>9.11</v>
       </c>
-      <c r="F120" s="29"/>
+      <c r="F120" s="30"/>
       <c r="G120" s="12" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="121" ht="36" spans="2:7">
@@ -4986,22 +5139,22 @@
         <v>39</v>
       </c>
       <c r="C121" s="10" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D121" s="12" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E121" s="19">
         <v>9.11</v>
       </c>
       <c r="F121" s="10"/>
       <c r="G121" s="12" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="122" ht="408" customHeight="1" spans="2:7">
       <c r="B122" s="13" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C122" s="14"/>
       <c r="D122" s="14"/>
@@ -5011,7 +5164,7 @@
     </row>
     <row r="123" spans="2:7">
       <c r="B123" s="15" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C123" s="16"/>
       <c r="D123" s="16"/>
@@ -5023,262 +5176,264 @@
       <c r="B124" s="9">
         <v>1</v>
       </c>
-      <c r="C124" s="30" t="s">
-        <v>297</v>
+      <c r="C124" s="26" t="s">
+        <v>294</v>
       </c>
       <c r="D124" s="12" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E124" s="19">
         <v>9.12</v>
       </c>
-      <c r="F124" s="30" t="s">
-        <v>299</v>
-      </c>
+      <c r="F124" s="30"/>
       <c r="G124" s="12" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="125" ht="36" spans="2:7">
       <c r="B125" s="9">
         <v>2</v>
       </c>
-      <c r="C125" s="31"/>
+      <c r="C125" s="28"/>
       <c r="D125" s="12" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="E125" s="19">
         <v>9.12</v>
       </c>
-      <c r="F125" s="31"/>
+      <c r="F125" s="30"/>
       <c r="G125" s="12" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="126" ht="24" spans="2:7">
       <c r="B126" s="9">
         <v>3</v>
       </c>
-      <c r="C126" s="31"/>
+      <c r="C126" s="28"/>
       <c r="D126" s="12" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="E126" s="19">
         <v>9.12</v>
       </c>
-      <c r="F126" s="31"/>
+      <c r="F126" s="30"/>
       <c r="G126" s="12" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="127" ht="72" spans="2:7">
       <c r="B127" s="9">
         <v>4</v>
       </c>
-      <c r="C127" s="31"/>
+      <c r="C127" s="28"/>
       <c r="D127" s="12" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="E127" s="19">
         <v>9.13</v>
       </c>
-      <c r="F127" s="31" t="s">
-        <v>306</v>
-      </c>
+      <c r="F127" s="30"/>
       <c r="G127" s="12" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="128" ht="192" spans="2:7">
       <c r="B128" s="9">
         <v>5</v>
       </c>
-      <c r="C128" s="32"/>
+      <c r="C128" s="29"/>
       <c r="D128" s="12" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="E128" s="19">
         <v>9.13</v>
       </c>
-      <c r="F128" s="31"/>
+      <c r="F128" s="30"/>
       <c r="G128" s="12" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="129" ht="84" spans="2:7">
       <c r="B129" s="9">
         <v>6</v>
       </c>
-      <c r="C129" s="30" t="s">
-        <v>310</v>
+      <c r="C129" s="26" t="s">
+        <v>305</v>
       </c>
       <c r="D129" s="12" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E129" s="19">
         <v>9.13</v>
       </c>
-      <c r="F129" s="31"/>
+      <c r="F129" s="30"/>
       <c r="G129" s="12" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="130" ht="48" spans="2:7">
       <c r="B130" s="9">
         <v>7</v>
       </c>
-      <c r="C130" s="32"/>
+      <c r="C130" s="29"/>
       <c r="D130" s="12" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="E130" s="19">
         <v>9.16</v>
       </c>
-      <c r="F130" s="31"/>
+      <c r="F130" s="30"/>
       <c r="G130" s="12" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="131" ht="60" spans="2:7">
       <c r="B131" s="9">
         <v>8</v>
       </c>
-      <c r="C131" s="30" t="s">
-        <v>315</v>
+      <c r="C131" s="26" t="s">
+        <v>310</v>
       </c>
       <c r="D131" s="12" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="E131" s="19">
         <v>9.17</v>
       </c>
-      <c r="F131" s="31"/>
+      <c r="F131" s="30"/>
       <c r="G131" s="12" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="132" ht="72" spans="2:7">
       <c r="B132" s="9">
         <v>9</v>
       </c>
-      <c r="C132" s="31"/>
+      <c r="C132" s="28"/>
       <c r="D132" s="12" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="E132" s="19">
         <v>9.17</v>
       </c>
-      <c r="F132" s="37"/>
+      <c r="F132" s="30"/>
       <c r="G132" s="12" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="133" ht="36" spans="2:7">
       <c r="B133" s="9">
         <v>10</v>
       </c>
-      <c r="C133" s="31"/>
+      <c r="C133" s="28"/>
       <c r="D133" s="12" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="E133" s="19">
         <v>9.18</v>
       </c>
-      <c r="F133" s="37"/>
+      <c r="F133" s="30"/>
       <c r="G133" s="12" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="134" ht="60" spans="2:7">
       <c r="B134" s="9">
         <v>11</v>
       </c>
-      <c r="C134" s="30" t="s">
-        <v>322</v>
+      <c r="C134" s="26" t="s">
+        <v>317</v>
       </c>
       <c r="D134" s="12" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="E134" s="19">
         <v>9.18</v>
       </c>
-      <c r="F134" s="38"/>
+      <c r="F134" s="30"/>
       <c r="G134" s="12" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="135" ht="36" spans="2:7">
       <c r="B135" s="9">
         <v>12</v>
       </c>
-      <c r="C135" s="32"/>
+      <c r="C135" s="28"/>
       <c r="D135" s="12" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E135" s="19">
         <v>9.18</v>
       </c>
-      <c r="F135" s="26" t="s">
-        <v>326</v>
-      </c>
+      <c r="F135" s="30"/>
       <c r="G135" s="12" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="136" spans="2:7">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="136" ht="24" spans="2:7">
       <c r="B136" s="9">
         <v>13</v>
       </c>
-      <c r="C136" s="30" t="s">
-        <v>328</v>
-      </c>
-      <c r="D136" s="12"/>
-      <c r="E136" s="19"/>
-      <c r="F136" s="28"/>
-      <c r="G136" s="12"/>
+      <c r="C136" s="28"/>
+      <c r="D136" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="E136" s="19">
+        <v>9.19</v>
+      </c>
+      <c r="F136" s="30"/>
+      <c r="G136" s="12" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="137" spans="2:7">
       <c r="B137" s="9">
         <v>14</v>
       </c>
-      <c r="C137" s="32"/>
-      <c r="D137" s="12"/>
-      <c r="E137" s="19"/>
-      <c r="F137" s="28"/>
+      <c r="C137" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="D137" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="E137" s="19">
+        <v>9.19</v>
+      </c>
+      <c r="F137" s="30"/>
       <c r="G137" s="12"/>
     </row>
     <row r="138" spans="2:7">
       <c r="B138" s="9">
         <v>15</v>
       </c>
-      <c r="C138" s="30" t="s">
-        <v>329</v>
-      </c>
+      <c r="C138" s="28"/>
       <c r="D138" s="12"/>
       <c r="E138" s="19"/>
-      <c r="F138" s="28"/>
+      <c r="F138" s="30"/>
       <c r="G138" s="12"/>
     </row>
     <row r="139" spans="2:7">
       <c r="B139" s="9">
         <v>16</v>
       </c>
-      <c r="C139" s="32"/>
+      <c r="C139" s="28" t="s">
+        <v>326</v>
+      </c>
       <c r="D139" s="12"/>
       <c r="E139" s="19"/>
-      <c r="F139" s="29"/>
+      <c r="F139" s="30"/>
       <c r="G139" s="12"/>
     </row>
     <row r="140" spans="2:7">
       <c r="B140" s="9">
         <v>17</v>
       </c>
-      <c r="C140" s="10"/>
-      <c r="D140" s="12"/>
+      <c r="C140" s="31"/>
+      <c r="D140" s="32"/>
       <c r="E140" s="19"/>
-      <c r="F140" s="26" t="s">
-        <v>330</v>
-      </c>
+      <c r="F140" s="30"/>
       <c r="G140" s="12"/>
     </row>
     <row r="141" spans="2:7">
@@ -5288,22 +5443,22 @@
       <c r="C141" s="10"/>
       <c r="D141" s="12"/>
       <c r="E141" s="19"/>
-      <c r="F141" s="29"/>
+      <c r="F141" s="30"/>
       <c r="G141" s="12"/>
     </row>
     <row r="142" ht="127" customHeight="1" spans="2:7">
       <c r="B142" s="13" t="s">
-        <v>331</v>
-      </c>
-      <c r="C142" s="33"/>
-      <c r="D142" s="33"/>
-      <c r="E142" s="33"/>
-      <c r="F142" s="33"/>
-      <c r="G142" s="39"/>
+        <v>327</v>
+      </c>
+      <c r="C142" s="14"/>
+      <c r="D142" s="14"/>
+      <c r="E142" s="14"/>
+      <c r="F142" s="14"/>
+      <c r="G142" s="21"/>
     </row>
     <row r="143" spans="2:7">
       <c r="B143" s="15" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C143" s="16"/>
       <c r="D143" s="16"/>
@@ -5311,17 +5466,23 @@
       <c r="F143" s="16"/>
       <c r="G143" s="22"/>
     </row>
-    <row r="144" spans="2:7">
+    <row r="144" ht="72" spans="2:7">
       <c r="B144" s="9">
         <v>1</v>
       </c>
-      <c r="C144" s="10"/>
-      <c r="D144" s="12"/>
-      <c r="E144" s="19"/>
-      <c r="F144" s="26" t="s">
-        <v>333</v>
-      </c>
-      <c r="G144" s="12"/>
+      <c r="C144" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="D144" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="E144" s="19">
+        <v>9.23</v>
+      </c>
+      <c r="F144" s="26"/>
+      <c r="G144" s="12" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="145" spans="2:7">
       <c r="B145" s="9">
@@ -5360,9 +5521,7 @@
       <c r="C148" s="10"/>
       <c r="D148" s="12"/>
       <c r="E148" s="19"/>
-      <c r="F148" s="26" t="s">
-        <v>334</v>
-      </c>
+      <c r="F148" s="26"/>
       <c r="G148" s="12"/>
     </row>
     <row r="149" spans="2:7">
@@ -5402,9 +5561,7 @@
       <c r="C152" s="10"/>
       <c r="D152" s="12"/>
       <c r="E152" s="19"/>
-      <c r="F152" s="26" t="s">
-        <v>335</v>
-      </c>
+      <c r="F152" s="26"/>
       <c r="G152" s="12"/>
     </row>
     <row r="153" spans="2:7">
@@ -5444,9 +5601,7 @@
       <c r="C156" s="10"/>
       <c r="D156" s="12"/>
       <c r="E156" s="19"/>
-      <c r="F156" s="26" t="s">
-        <v>336</v>
-      </c>
+      <c r="F156" s="26"/>
       <c r="G156" s="12"/>
     </row>
     <row r="157" spans="2:7">
@@ -5486,9 +5641,7 @@
       <c r="C160" s="10"/>
       <c r="D160" s="12"/>
       <c r="E160" s="19"/>
-      <c r="F160" s="26" t="s">
-        <v>337</v>
-      </c>
+      <c r="F160" s="26"/>
       <c r="G160" s="12"/>
     </row>
     <row r="161" spans="2:7">
@@ -5502,18 +5655,18 @@
       <c r="G161" s="12"/>
     </row>
     <row r="162" spans="2:7">
-      <c r="B162" s="34" t="s">
-        <v>170</v>
-      </c>
-      <c r="C162" s="35"/>
-      <c r="D162" s="35"/>
-      <c r="E162" s="35"/>
-      <c r="F162" s="35"/>
+      <c r="B162" s="31" t="s">
+        <v>331</v>
+      </c>
+      <c r="C162" s="33"/>
+      <c r="D162" s="33"/>
+      <c r="E162" s="33"/>
+      <c r="F162" s="33"/>
       <c r="G162" s="40"/>
     </row>
     <row r="163" spans="2:7">
       <c r="B163" s="15" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="C163" s="16"/>
       <c r="D163" s="16"/>
@@ -5523,7 +5676,7 @@
     </row>
     <row r="165" spans="2:7">
       <c r="B165" s="15" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C165" s="16"/>
       <c r="D165" s="16"/>
@@ -5538,9 +5691,7 @@
       <c r="C166" s="10"/>
       <c r="D166" s="12"/>
       <c r="E166" s="19"/>
-      <c r="F166" s="26" t="s">
-        <v>340</v>
-      </c>
+      <c r="F166" s="26"/>
       <c r="G166" s="12"/>
     </row>
     <row r="167" spans="2:7">
@@ -5589,11 +5740,11 @@
       <c r="D171" s="35"/>
       <c r="E171" s="35"/>
       <c r="F171" s="35"/>
-      <c r="G171" s="40"/>
+      <c r="G171" s="41"/>
     </row>
     <row r="172" spans="2:7">
       <c r="B172" s="15" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="C172" s="16"/>
       <c r="D172" s="16"/>
@@ -5609,11 +5760,43 @@
     </row>
     <row r="176" spans="3:3">
       <c r="C176" s="36" t="s">
-        <v>342</v>
+        <v>335</v>
+      </c>
+    </row>
+    <row r="180" spans="2:7">
+      <c r="B180" s="15" t="s">
+        <v>336</v>
+      </c>
+      <c r="C180" s="16"/>
+      <c r="D180" s="16"/>
+      <c r="E180" s="16"/>
+      <c r="F180" s="16"/>
+      <c r="G180" s="22"/>
+    </row>
+    <row r="181" ht="409.5" spans="3:7">
+      <c r="C181" s="37"/>
+      <c r="D181" s="38" t="s">
+        <v>337</v>
+      </c>
+      <c r="E181" s="38" t="s">
+        <v>338</v>
+      </c>
+      <c r="F181" s="37"/>
+      <c r="G181" s="30" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="182" ht="409.5" spans="3:7">
+      <c r="C182" s="39"/>
+      <c r="D182" s="38"/>
+      <c r="E182" s="38"/>
+      <c r="F182" s="39"/>
+      <c r="G182" s="30" t="s">
+        <v>340</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="53">
+  <mergeCells count="51">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B15:G15"/>
@@ -5632,6 +5815,7 @@
     <mergeCell ref="B74:G74"/>
     <mergeCell ref="B122:G122"/>
     <mergeCell ref="B123:G123"/>
+    <mergeCell ref="C140:D140"/>
     <mergeCell ref="B142:G142"/>
     <mergeCell ref="B143:G143"/>
     <mergeCell ref="B162:G162"/>
@@ -5639,6 +5823,7 @@
     <mergeCell ref="B165:G165"/>
     <mergeCell ref="B171:G171"/>
     <mergeCell ref="B172:G172"/>
+    <mergeCell ref="B180:G180"/>
     <mergeCell ref="C4:C8"/>
     <mergeCell ref="C75:C77"/>
     <mergeCell ref="C78:C80"/>
@@ -5650,22 +5835,18 @@
     <mergeCell ref="C124:C128"/>
     <mergeCell ref="C129:C130"/>
     <mergeCell ref="C131:C133"/>
-    <mergeCell ref="C134:C135"/>
-    <mergeCell ref="C136:C137"/>
-    <mergeCell ref="C138:C139"/>
-    <mergeCell ref="F106:F111"/>
-    <mergeCell ref="F112:F116"/>
-    <mergeCell ref="F117:F120"/>
-    <mergeCell ref="F124:F126"/>
-    <mergeCell ref="F127:F131"/>
-    <mergeCell ref="F135:F139"/>
-    <mergeCell ref="F140:F141"/>
+    <mergeCell ref="C134:C136"/>
+    <mergeCell ref="C137:C139"/>
+    <mergeCell ref="C181:C182"/>
+    <mergeCell ref="D181:D182"/>
+    <mergeCell ref="E181:E182"/>
     <mergeCell ref="F144:F147"/>
     <mergeCell ref="F148:F151"/>
     <mergeCell ref="F152:F155"/>
     <mergeCell ref="F156:F159"/>
     <mergeCell ref="F160:F161"/>
     <mergeCell ref="F166:F170"/>
+    <mergeCell ref="F181:F182"/>
     <mergeCell ref="G4:G8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5692,7 +5873,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -5700,24 +5881,24 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>345</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -5742,10 +5923,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -5753,7 +5934,7 @@
     <row r="8" spans="1:4">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -5761,7 +5942,7 @@
     <row r="9" spans="1:4">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -5769,7 +5950,7 @@
     <row r="10" spans="1:4">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>

</xml_diff>

<commit_message>
leetcode: add greedy subjects
</commit_message>
<xml_diff>
--- a/leetcode路线.xlsx
+++ b/leetcode路线.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="357">
   <si>
     <t>从9月23日开始保持每天2个题目,还剩113题,写57天,2024年11月19日可刷完leetcode第一遍
 慢慢做,不要慌,每个题都要搞懂,不要水,静下心来</t>
@@ -1693,9 +1693,24 @@
   <si>
     <t>js:
 本来很快就能写出来!结果,被sort摆了一道,气死我了!!!
-g.sort()：按照字符串的Unicode码点顺序进行排序。因此结果可能并不是按数值的大小进行排序。
+1.g.sort()：按照字符串的Unicode码点顺序进行排序。因此结果可能并不是按数值的大小进行排序。
 g.sort((a, b) =&gt; a - b)：带有比较函数的排序方式，能够按照数值的大小对数组元素进行排序。
-    (a, b) =&gt; a - b 是一个比较函数，当 a - b 为负数时，a 会排在 b 之前，这就能保证数字按升序排列。</t>
+    (a, b) =&gt; a - b 是一个比较函数，当 a - b 为负数时，a 会排在 b 之前，这就能保证数字按升序排列。
+2.技巧: 使用一个for循环控制</t>
+  </si>
+  <si>
+    <t>376. 摆动序列</t>
+  </si>
+  <si>
+    <t>js:
+这个题三种情况难考虑全!!思路还没捋清楚..</t>
+  </si>
+  <si>
+    <t>53. 最大子数组和</t>
+  </si>
+  <si>
+    <t>js:
+常识不好想,需要累计经验,代码比较好写</t>
   </si>
   <si>
     <t>9.23总结:
@@ -3113,10 +3128,10 @@
   <sheetPr/>
   <dimension ref="A1:G182"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G144" sqref="G144"/>
+      <selection pane="bottomLeft" activeCell="G146" sqref="G146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="16.5" outlineLevelCol="6"/>
@@ -5466,7 +5481,7 @@
       <c r="F143" s="16"/>
       <c r="G143" s="22"/>
     </row>
-    <row r="144" ht="72" spans="2:7">
+    <row r="144" ht="84" spans="2:7">
       <c r="B144" s="9">
         <v>1</v>
       </c>
@@ -5484,25 +5499,41 @@
         <v>330</v>
       </c>
     </row>
-    <row r="145" spans="2:7">
+    <row r="145" ht="24" spans="2:7">
       <c r="B145" s="9">
         <v>2</v>
       </c>
-      <c r="C145" s="10"/>
-      <c r="D145" s="12"/>
-      <c r="E145" s="19"/>
+      <c r="C145" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="D145" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="E145" s="19">
+        <v>9.24</v>
+      </c>
       <c r="F145" s="28"/>
-      <c r="G145" s="12"/>
-    </row>
-    <row r="146" spans="2:7">
+      <c r="G145" s="12" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="146" ht="24" spans="2:7">
       <c r="B146" s="9">
         <v>3</v>
       </c>
-      <c r="C146" s="10"/>
-      <c r="D146" s="12"/>
-      <c r="E146" s="19"/>
+      <c r="C146" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="D146" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="E146" s="19">
+        <v>9.24</v>
+      </c>
       <c r="F146" s="28"/>
-      <c r="G146" s="12"/>
+      <c r="G146" s="12" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="147" spans="2:7">
       <c r="B147" s="9">
@@ -5656,7 +5687,7 @@
     </row>
     <row r="162" spans="2:7">
       <c r="B162" s="31" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="C162" s="33"/>
       <c r="D162" s="33"/>
@@ -5666,7 +5697,7 @@
     </row>
     <row r="163" spans="2:7">
       <c r="B163" s="15" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="C163" s="16"/>
       <c r="D163" s="16"/>
@@ -5676,7 +5707,7 @@
     </row>
     <row r="165" spans="2:7">
       <c r="B165" s="15" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="C165" s="16"/>
       <c r="D165" s="16"/>
@@ -5744,7 +5775,7 @@
     </row>
     <row r="172" spans="2:7">
       <c r="B172" s="15" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="C172" s="16"/>
       <c r="D172" s="16"/>
@@ -5760,12 +5791,12 @@
     </row>
     <row r="176" spans="3:3">
       <c r="C176" s="36" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
     </row>
     <row r="180" spans="2:7">
       <c r="B180" s="15" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="C180" s="16"/>
       <c r="D180" s="16"/>
@@ -5776,14 +5807,14 @@
     <row r="181" ht="409.5" spans="3:7">
       <c r="C181" s="37"/>
       <c r="D181" s="38" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="E181" s="38" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="F181" s="37"/>
       <c r="G181" s="30" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
     </row>
     <row r="182" ht="409.5" spans="3:7">
@@ -5792,7 +5823,7 @@
       <c r="E182" s="38"/>
       <c r="F182" s="39"/>
       <c r="G182" s="30" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>
@@ -5873,7 +5904,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -5881,24 +5912,24 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -5923,10 +5954,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -5934,7 +5965,7 @@
     <row r="8" spans="1:4">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -5942,7 +5973,7 @@
     <row r="9" spans="1:4">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -5950,7 +5981,7 @@
     <row r="10" spans="1:4">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>

</xml_diff>